<commit_message>
Created Prototype Stats System with basic string expressions
expression examples:
p1.hp+10
boss.hp-15
p2.spd+10
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Tests/EditModeTests/TestData/TestCardDatabase.xlsx
+++ b/Assets/Scripts/Tests/EditModeTests/TestData/TestCardDatabase.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unity Projects\VirtualDeck\Assets\Scripts\Tests\EditModeTests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFC0C99-F896-4311-A4D2-063B586E4620}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDC0803-E3A6-41C2-8148-0FA0C4914B0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="915" windowWidth="21585" windowHeight="11385" xr2:uid="{F2C55B00-21E3-46B1-ADD7-025CF5B3F2CE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F2C55B00-21E3-46B1-ADD7-025CF5B3F2CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Cards" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>Title</t>
   </si>
@@ -61,6 +62,18 @@
   </si>
   <si>
     <t>Card3 Action</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>half-heart</t>
+  </si>
+  <si>
+    <t>CardType</t>
+  </si>
+  <si>
+    <t>Skill</t>
   </si>
 </sst>
 </file>
@@ -412,15 +425,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71E7FDE-B8FF-4097-9BD1-1D16559BBB7E}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,8 +443,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -441,8 +460,14 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -452,8 +477,14 @@
       <c r="C3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -462,6 +493,78 @@
       </c>
       <c r="C4">
         <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF085B5-7A73-4BF1-AA99-D4FF33F09D3B}">
+  <dimension ref="A2:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16:E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>